<commit_message>
Enchainement operateurs MyScadeGenerator + Destruction fichier existant
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.5.xlsx
+++ b/Matrix-Usecase-V1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\S2\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCF0BED-8E60-4478-802C-7BF913726F50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96697C82-F198-49B8-90B3-8E6DD2C7C2E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{810DAD72-4B4F-4F6F-8B91-F7F08FE9DCA9}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Transition Table" sheetId="1" r:id="rId1"/>
     <sheet name="Change Mode" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -795,36 +795,6 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1364,13 +1334,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1382,6 +1345,13 @@
           <color indexed="64"/>
         </top>
         <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -1403,6 +1373,36 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1500,23 +1500,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC0F6965-AA70-4176-99DC-18B9F3AB6D46}" name="Tableau3" displayName="Tableau3" ref="A1:N27" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC0F6965-AA70-4176-99DC-18B9F3AB6D46}" name="Tableau3" displayName="Tableau3" ref="A1:N27" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:N27" xr:uid="{F04C33A3-CE71-42CF-9EBA-2F522A833DC5}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{DBB20545-9B04-47E0-BFB2-48E387D068E8}" name="Start Mode" dataDxfId="16" dataCellStyle="Note"/>
-    <tableColumn id="2" xr3:uid="{5D221613-F7A1-4A4D-8692-94F761C7A824}" name="Change?" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{52AA0E47-7E0A-46FD-B39D-ADAFBE7B4895}" name="Weather" dataDxfId="14" dataCellStyle="Note"/>
-    <tableColumn id="4" xr3:uid="{54EF9241-EA7F-4DB0-B102-32329872E6ED}" name="W Problem?" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{ED94291C-8728-4929-ACA1-076A53C83258}" name="Road" dataDxfId="12" dataCellStyle="Note"/>
-    <tableColumn id="6" xr3:uid="{2DF720B2-03F7-4881-AF33-A624177DAB00}" name="R Problem?" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{A9130A10-63C9-4C82-AD04-DDA6B3D98AE5}" name="Traffic" dataDxfId="10" dataCellStyle="Note"/>
-    <tableColumn id="8" xr3:uid="{27543BA1-519F-466C-B087-680289BE07B0}" name="T Problem?" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{9DE7C9B8-B630-4165-BBA3-6C1B51CBB0A3}" name="Vehicle" dataDxfId="8" dataCellStyle="Note"/>
-    <tableColumn id="10" xr3:uid="{0757CCA3-4C91-47A9-9128-539AF5A867FB}" name="V Problem?" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{B77A2194-8A21-4496-B7DA-036E2A1B4C1D}" name="Human" dataDxfId="6" dataCellStyle="Note"/>
-    <tableColumn id="12" xr3:uid="{EA1FBC6C-0961-4BF7-A042-5EB498CCFCAC}" name="H Problem?" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{D33B3DB1-78F4-4817-A8D2-170B3306CF88}" name="Final Mode" dataDxfId="4" dataCellStyle="Sortie"/>
-    <tableColumn id="14" xr3:uid="{10AD2450-C116-4B7F-A2AB-E871610EDD97}" name="Equation" dataDxfId="3" dataCellStyle="Entrée"/>
+    <tableColumn id="1" xr3:uid="{DBB20545-9B04-47E0-BFB2-48E387D068E8}" name="Start Mode" dataDxfId="13" dataCellStyle="Note"/>
+    <tableColumn id="2" xr3:uid="{5D221613-F7A1-4A4D-8692-94F761C7A824}" name="Change?" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{52AA0E47-7E0A-46FD-B39D-ADAFBE7B4895}" name="Weather" dataDxfId="11" dataCellStyle="Note"/>
+    <tableColumn id="4" xr3:uid="{54EF9241-EA7F-4DB0-B102-32329872E6ED}" name="W Problem?" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{ED94291C-8728-4929-ACA1-076A53C83258}" name="Road" dataDxfId="9" dataCellStyle="Note"/>
+    <tableColumn id="6" xr3:uid="{2DF720B2-03F7-4881-AF33-A624177DAB00}" name="R Problem?" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{A9130A10-63C9-4C82-AD04-DDA6B3D98AE5}" name="Traffic" dataDxfId="7" dataCellStyle="Note"/>
+    <tableColumn id="8" xr3:uid="{27543BA1-519F-466C-B087-680289BE07B0}" name="T Problem?" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{9DE7C9B8-B630-4165-BBA3-6C1B51CBB0A3}" name="Vehicle" dataDxfId="5" dataCellStyle="Note"/>
+    <tableColumn id="10" xr3:uid="{0757CCA3-4C91-47A9-9128-539AF5A867FB}" name="V Problem?" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{B77A2194-8A21-4496-B7DA-036E2A1B4C1D}" name="Human" dataDxfId="3" dataCellStyle="Note"/>
+    <tableColumn id="12" xr3:uid="{EA1FBC6C-0961-4BF7-A042-5EB498CCFCAC}" name="H Problem?" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{D33B3DB1-78F4-4817-A8D2-170B3306CF88}" name="Final Mode" dataDxfId="1" dataCellStyle="Sortie"/>
+    <tableColumn id="14" xr3:uid="{10AD2450-C116-4B7F-A2AB-E871610EDD97}" name="Equation" dataDxfId="0" dataCellStyle="Entrée"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -82623,7 +82623,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82951,7 +82951,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>0</v>
       </c>
@@ -83863,7 +83863,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576 D1:D1048576 F1:F1048576 H1:H1048576 J1:J1048576 L1:L1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="IDEM">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="IDEM">
       <formula>NOT(ISERROR(SEARCH("IDEM",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Inclusion Repository Mallet - ERROR ON BDD
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.5.xlsx
+++ b/Matrix-Usecase-V1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\S2\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96697C82-F198-49B8-90B3-8E6DD2C7C2E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4D1E24-9DDF-4E98-B672-A54BEA6C1DD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{810DAD72-4B4F-4F6F-8B91-F7F08FE9DCA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{810DAD72-4B4F-4F6F-8B91-F7F08FE9DCA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Transition Table" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24813" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24814" uniqueCount="70">
   <si>
     <t>Manual</t>
   </si>
@@ -1821,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAF2099-6733-454A-91BF-8E7F44F23A38}">
   <dimension ref="A1:G3512"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82608,7 +82608,9 @@
       <c r="F3512" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G3512" s="4"/>
+      <c r="G3512" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -82622,8 +82624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED3CFF5-6A34-494B-A07C-9BAB108935BD}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>